<commit_message>
Reajustado numeros y añadido descripcciones
</commit_message>
<xml_diff>
--- a/ponderaciones/Ponderaciones.xlsx
+++ b/ponderaciones/Ponderaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Universidad\3\PINF\CalculadoraCO2\ponderaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE0DF24-269E-4E7B-BAC3-6C48E9A05CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2893719F-E89F-4ABE-A260-8A1B772E7D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2220" windowWidth="29040" windowHeight="15720" xr2:uid="{1F3419FC-22DA-443A-A229-AEE1317CE497}"/>
   </bookViews>
@@ -629,10 +629,10 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="C3">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -643,10 +643,10 @@
         <v>8</v>
       </c>
       <c r="B4">
+        <v>0.09</v>
+      </c>
+      <c r="C4">
         <v>0.04</v>
-      </c>
-      <c r="C4">
-        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -657,10 +657,10 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0.18</v>
+        <v>0.05</v>
       </c>
       <c r="C5">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -676,7 +676,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.15</v>
+        <v>0.19</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
@@ -687,7 +687,7 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>0.9</v>
+        <v>0.08</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
@@ -711,7 +711,7 @@
         <v>5</v>
       </c>
       <c r="B11">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>